<commit_message>
I did a whole bunch with updates
</commit_message>
<xml_diff>
--- a/testing/ToDo.xlsx
+++ b/testing/ToDo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumenty\plocha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumenty\okurz\Github\yt-dl\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99844B85-450A-4958-BCC4-DE0F2702810E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A10D37E-0E90-4758-9053-77D11AF236E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-9480" windowWidth="29040" windowHeight="15840" xr2:uid="{0FD08222-D3DA-4E09-8896-7B7DFE2FA52D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="76">
   <si>
     <t>GUI:</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Subs</t>
   </si>
   <si>
-    <t>Sub download dos not support playlist download</t>
-  </si>
-  <si>
     <t>if supported in yt-dl than with more loops possible</t>
   </si>
   <si>
@@ -201,9 +198,6 @@
     <t>to see waht ffmpeg version I'm using</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
     <t>CLI:</t>
   </si>
   <si>
@@ -217,6 +211,57 @@
   </si>
   <si>
     <t>I wrote sub download and than let it be a black box</t>
+  </si>
+  <si>
+    <t>2.1.8</t>
+  </si>
+  <si>
+    <t>2.1.9</t>
+  </si>
+  <si>
+    <t>GUI redesign</t>
+  </si>
+  <si>
+    <t>Even tho 2.1.8 is not done it already needs to be planned</t>
+  </si>
+  <si>
+    <t>Audio,Subs</t>
+  </si>
+  <si>
+    <t>Audio &amp; Sub tab does not have to exist</t>
+  </si>
+  <si>
+    <t>It can all be download tab with radio buttons</t>
+  </si>
+  <si>
+    <t>Official Hubz design Edition</t>
+  </si>
+  <si>
+    <t>Please and thank you mister hubz the designer</t>
+  </si>
+  <si>
+    <t>Sub download does not support playlist download</t>
+  </si>
+  <si>
+    <t>Reencode</t>
+  </si>
+  <si>
+    <t>Ree dowes not support whole folder re-encode</t>
+  </si>
+  <si>
+    <t>depends on subs playlist downlosad for now</t>
+  </si>
+  <si>
+    <t>If video already exists there is now way to press y/n</t>
+  </si>
+  <si>
+    <t>Auto numbering?</t>
+  </si>
+  <si>
+    <t>AutoUpd</t>
+  </si>
+  <si>
+    <t>Autoupdate on start updates first but does not start UI</t>
   </si>
 </sst>
 </file>
@@ -277,15 +322,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="9">
     <dxf>
       <font>
         <color theme="4" tint="-0.24994659260841701"/>
@@ -294,53 +341,6 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="0.39994506668294322"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -356,11 +356,38 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="5" tint="-0.24994659260841701"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="0.39994506668294322"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -386,359 +413,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="0.39994506668294322"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="0.39994506668294322"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="0.39994506668294322"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1052,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD1110F-3924-4260-99AB-6C82287FA024}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,36 +771,18 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -1133,10 +794,10 @@
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>10</v>
@@ -1144,66 +805,64 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>20</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>19</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>10</v>
@@ -1211,43 +870,43 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>10</v>
@@ -1255,22 +914,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>10</v>
@@ -1278,22 +937,20 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>10</v>
@@ -1301,56 +958,50 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>23</v>
@@ -1359,10 +1010,10 @@
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>10</v>
@@ -1370,22 +1021,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>10</v>
@@ -1393,20 +1044,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>18</v>
-      </c>
-      <c r="B16" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>10</v>
@@ -1414,20 +1067,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>11</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C17" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>10</v>
@@ -1435,20 +1090,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>12</v>
-      </c>
-      <c r="B18" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C18" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>10</v>
@@ -1456,46 +1113,68 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>10</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>56</v>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>13</v>
-      </c>
-      <c r="B21" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C21" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>10</v>
@@ -1503,36 +1182,202 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>17</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>13</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>16</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="2" t="s">
+      <c r="E26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="2" t="s">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>2</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>3</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+  <conditionalFormatting sqref="B1 B33:B1048576 B3:B31">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>"Canceled"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
-      <formula>"Canceled"</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1 C33:C1048576 C3:C31">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"low"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"high"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+      <formula>"high"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+      <formula>"highest"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="G1 G33:G1048576 G3:G31">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Windows"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33:A1048576 A3:A31 A1">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1543,31 +1388,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
-      <formula>"highest"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
-      <formula>"high"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
-      <formula>"high"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
-      <formula>"medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
-      <formula>"medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
-      <formula>"low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Windows"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
most of the saving+settings, really ugly code
</commit_message>
<xml_diff>
--- a/testing/ToDo.xlsx
+++ b/testing/ToDo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumenty\okurz\Github\yt-dl\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A10D37E-0E90-4758-9053-77D11AF236E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCECEF1D-D5C7-433A-8B2E-D863606B456E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-9480" windowWidth="29040" windowHeight="15840" xr2:uid="{0FD08222-D3DA-4E09-8896-7B7DFE2FA52D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="77">
   <si>
     <t>GUI:</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Shown in the status, will throw a message box</t>
   </si>
   <si>
-    <t>Button than opens you downloads forder</t>
-  </si>
-  <si>
     <t>Useful as fuck</t>
   </si>
   <si>
@@ -246,9 +243,6 @@
     <t>Reencode</t>
   </si>
   <si>
-    <t>Ree dowes not support whole folder re-encode</t>
-  </si>
-  <si>
     <t>depends on subs playlist downlosad for now</t>
   </si>
   <si>
@@ -262,6 +256,15 @@
   </si>
   <si>
     <t>Autoupdate on start updates first but does not start UI</t>
+  </si>
+  <si>
+    <t>Ree does not support whole folder re-encode</t>
+  </si>
+  <si>
+    <t>Button that opens your downloads forder</t>
+  </si>
+  <si>
+    <t>Posponed</t>
   </si>
 </sst>
 </file>
@@ -332,7 +335,105 @@
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="0.39994506668294322"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="4" tint="-0.24994659260841701"/>
@@ -734,12 +835,13 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="62.42578125" bestFit="1" customWidth="1"/>
@@ -772,7 +874,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -835,13 +937,13 @@
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>10</v>
@@ -856,13 +958,13 @@
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>10</v>
@@ -877,13 +979,13 @@
         <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>10</v>
@@ -939,7 +1041,9 @@
       <c r="A11" s="2">
         <v>19</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
@@ -947,10 +1051,10 @@
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>10</v>
@@ -960,15 +1064,17 @@
       <c r="A12" s="2">
         <v>22</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
@@ -979,21 +1085,23 @@
       <c r="A13" s="2">
         <v>5</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1004,16 +1112,16 @@
         <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>10</v>
@@ -1027,16 +1135,16 @@
         <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>10</v>
@@ -1050,16 +1158,16 @@
         <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>10</v>
@@ -1073,16 +1181,16 @@
         <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>10</v>
@@ -1096,16 +1204,16 @@
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>10</v>
@@ -1116,19 +1224,19 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>10</v>
@@ -1142,16 +1250,16 @@
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>10</v>
@@ -1165,16 +1273,16 @@
         <v>8</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>10</v>
@@ -1186,16 +1294,16 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>10</v>
@@ -1207,16 +1315,16 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>10</v>
@@ -1224,7 +1332,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1233,16 +1341,16 @@
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>10</v>
@@ -1254,16 +1362,16 @@
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>10</v>
@@ -1271,7 +1379,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1291,10 +1399,10 @@
         <v>10</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>10</v>
@@ -1309,13 +1417,13 @@
         <v>15</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>10</v>
@@ -1327,16 +1435,16 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>10</v>
@@ -1344,40 +1452,40 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1 B33:B1048576 B3:B31">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
       <formula>"Canceled"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1 C33:C1048576 C3:C31">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
       <formula>"low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>"medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>"medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
       <formula>"high"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>"high"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>"highest"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1 G33:G1048576 G3:G31">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"Windows"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:A1048576 A3:A31 A1">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1388,6 +1496,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"PosPoned"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Bolding issues that need to be resolved before launching
</commit_message>
<xml_diff>
--- a/testing/ToDo.xlsx
+++ b/testing/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumenty\okurz\Github\yt-dl\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCECEF1D-D5C7-433A-8B2E-D863606B456E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BAC0C6-22B9-4408-9437-38468E3882D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-9480" windowWidth="29040" windowHeight="15840" xr2:uid="{0FD08222-D3DA-4E09-8896-7B7DFE2FA52D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="84">
   <si>
     <t>GUI:</t>
   </si>
@@ -265,6 +265,27 @@
   </si>
   <si>
     <t>Posponed</t>
+  </si>
+  <si>
+    <t>Not Autoupdating will lead to videos not downloading.</t>
+  </si>
+  <si>
+    <t>Launch</t>
+  </si>
+  <si>
+    <t>Find a way to lauch without a cmd poping up and in venv</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>Is A tab hideable? Or enable diable-ble</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Bold issues need to de bealt with before launching</t>
   </si>
 </sst>
 </file>
@@ -325,17 +346,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="10">
     <dxf>
       <font>
         <color theme="5" tint="-0.24994659260841701"/>
@@ -343,94 +367,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="0.39994506668294322"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -832,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD1110F-3924-4260-99AB-6C82287FA024}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +785,7 @@
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -872,17 +808,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -905,7 +841,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -927,119 +863,117 @@
       <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="I5" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>21</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="G6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>20</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="G7" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>18</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="G8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>23</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>24</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>3</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>8</v>
@@ -1048,88 +982,88 @@
         <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="G12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>22</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>6</v>
-      </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
@@ -1138,21 +1072,21 @@
         <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
@@ -1164,10 +1098,10 @@
         <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>10</v>
@@ -1175,7 +1109,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
@@ -1184,13 +1118,13 @@
         <v>22</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>10</v>
@@ -1198,7 +1132,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>8</v>
@@ -1210,10 +1144,10 @@
         <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>10</v>
@@ -1221,10 +1155,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>22</v>
@@ -1233,10 +1167,10 @@
         <v>10</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>10</v>
@@ -1244,22 +1178,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>10</v>
@@ -1267,22 +1201,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>10</v>
@@ -1290,67 +1224,85 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>17</v>
-      </c>
-      <c r="B23" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C23" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>53</v>
+      <c r="A24" s="2">
+        <v>11</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>10</v>
@@ -1358,133 +1310,180 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>13</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>0</v>
+      <c r="D28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="2" t="s">
+      <c r="D32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="G32" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
         <v>2</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="4" t="s">
+      <c r="B33" s="2"/>
+      <c r="C33" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G30" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="G33" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
         <v>3</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="4" t="s">
+      <c r="B34" s="2"/>
+      <c r="C34" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="4" t="s">
+      <c r="D34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F34" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G34" s="4" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B33:B1048576 B3:B31">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+  <conditionalFormatting sqref="B1 B36:B1048576 B3:B34">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"Canceled"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1 C33:C1048576 C3:C31">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+  <conditionalFormatting sqref="C1 C36:C1048576 C3:C34">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"high"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"high"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"highest"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1 G33:G1048576 G3:G31">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+  <conditionalFormatting sqref="G1 G36:G1048576 G3:G34 H10">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Windows"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A33:A1048576 A3:A31 A1">
+  <conditionalFormatting sqref="A36:A1048576 A3:A34 A1">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
fogot so save excel
</commit_message>
<xml_diff>
--- a/testing/ToDo.xlsx
+++ b/testing/ToDo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\okurz\Documents\Github\yt-dl\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumenty\okurz\Github\yt-dl\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31A2989-74A3-4B77-A882-7D3A04A694F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFB955D-ABDE-4184-832D-006267016ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FD08222-D3DA-4E09-8896-7B7DFE2FA52D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FD08222-D3DA-4E09-8896-7B7DFE2FA52D}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="84">
   <si>
     <t>GUI:</t>
   </si>
@@ -350,123 +350,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="0.39994506668294322"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="0.39994506668294322"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -636,7 +522,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -935,7 +821,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:C35"/>
+      <selection activeCell="A8" sqref="A8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,23 +960,25 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="8">
         <v>18</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1637,15 +1525,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1 B36:B1048576 B3:B34">
-    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="28" operator="equal">
       <formula>"Canceled"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="29" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1 G36:G1048576 G3:G34 H10">
-    <cfRule type="cellIs" dxfId="25" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
       <formula>"Windows"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1662,7 +1550,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="24" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="19" operator="equal">
       <formula>"PosPoned"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Feature complete on Win
</commit_message>
<xml_diff>
--- a/testing/ToDo.xlsx
+++ b/testing/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumenty\okurz\Github\yt-dl\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFB955D-ABDE-4184-832D-006267016ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C259BF-4C09-47B0-A319-CDBAD76671A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FD08222-D3DA-4E09-8896-7B7DFE2FA52D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="85">
   <si>
     <t>GUI:</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>threading to make drowing to a textbox not freeze</t>
+  </si>
+  <si>
+    <t>I drop venv support</t>
   </si>
 </sst>
 </file>
@@ -337,13 +340,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -821,14 +823,14 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:G8"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="62.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="57" bestFit="1" customWidth="1"/>
@@ -842,7 +844,7 @@
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -918,110 +920,118 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="7">
         <v>21</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="7">
         <v>20</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>18</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="G8" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>23</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="F9" s="7"/>
+      <c r="G9" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>24</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5" t="s">
+      <c r="F10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1317,7 +1327,7 @@
       <c r="G23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K23" s="9"/>
+      <c r="K23" s="8"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">

</xml_diff>

<commit_message>
gui5 mp3 + clean up
</commit_message>
<xml_diff>
--- a/testing/ToDo.xlsx
+++ b/testing/ToDo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumenty\okurz\Github\yt-dl\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C259BF-4C09-47B0-A319-CDBAD76671A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785D4444-8F60-48E7-A9D1-521D003B93F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FD08222-D3DA-4E09-8896-7B7DFE2FA52D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="89">
   <si>
     <t>GUI:</t>
   </si>
@@ -280,13 +280,25 @@
   </si>
   <si>
     <t>I drop venv support</t>
+  </si>
+  <si>
+    <t>add mp3/wave audio only option</t>
+  </si>
+  <si>
+    <t>drag and drop in re-encode</t>
+  </si>
+  <si>
+    <t>bring config file up to date with gui5</t>
+  </si>
+  <si>
+    <t>bring feature set up to date with gui5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,6 +311,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -354,7 +373,7 @@
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="40">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -376,15 +395,109 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
+      <font>
+        <color theme="7" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
           <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color theme="7" tint="0.39994506668294322"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.24994659260841701"/>
       </font>
       <fill>
         <patternFill>
@@ -394,6 +507,57 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="7" tint="-0.24994659260841701"/>
       </font>
       <fill>
@@ -427,25 +591,130 @@
         <color theme="5" tint="-0.24994659260841701"/>
       </font>
       <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
+      <font>
+        <color theme="7" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
           <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color theme="7" tint="0.39994506668294322"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -820,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD1110F-3924-4260-99AB-6C82287FA024}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,9 +1188,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>21</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>8</v>
@@ -942,9 +1211,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
-        <v>20</v>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>8</v>
@@ -966,8 +1235,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
-        <v>18</v>
+      <c r="A8" s="2">
+        <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>8</v>
@@ -989,8 +1258,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>23</v>
+      <c r="A9" s="2">
+        <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>8</v>
@@ -1010,8 +1279,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>24</v>
+      <c r="A10" s="2">
+        <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>38</v>
@@ -1037,7 +1306,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>8</v>
@@ -1060,7 +1329,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>8</v>
@@ -1083,7 +1352,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
@@ -1106,7 +1375,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>8</v>
@@ -1127,7 +1396,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
@@ -1150,7 +1419,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
@@ -1173,7 +1442,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
@@ -1196,7 +1465,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>8</v>
@@ -1219,7 +1488,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>8</v>
@@ -1242,7 +1511,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>8</v>
@@ -1265,7 +1534,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>38</v>
@@ -1288,17 +1557,19 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>25</v>
-      </c>
-      <c r="B22" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
@@ -1307,7 +1578,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>8</v>
@@ -1331,7 +1602,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>8</v>
@@ -1354,161 +1625,157 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>12</v>
-      </c>
-      <c r="B25" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C25" s="2" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>17</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>10</v>
+      <c r="A26" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>53</v>
+      <c r="A27" s="2">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>16</v>
+      <c r="A29" s="4">
+        <v>3</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>57</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="F29" s="2"/>
       <c r="G29" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4">
+        <v>4</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>1</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>2</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>66</v>
+        <v>15</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>10</v>
@@ -1516,39 +1783,114 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="2" t="s">
+      <c r="D35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>4</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2" t="s">
+      <c r="F36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>5</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>7</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>8</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B36:B1048576 B3:B34">
-    <cfRule type="cellIs" dxfId="15" priority="28" operator="equal">
-      <formula>"Canceled"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="29" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1 G36:G1048576 G3:G34 H10">
-    <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="15" priority="20" operator="equal">
       <formula>"Windows"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A1048576 A1">
-    <cfRule type="colorScale" priority="36">
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="colorScale" priority="150">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1559,52 +1901,35 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="12" priority="19" operator="equal">
-      <formula>"PosPoned"</formula>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+      <formula>"highest"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+      <formula>"high"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+      <formula>"medium"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
-      <formula>"medium"</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
+      <formula>"PosPoned"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
-      <formula>"medium"</formula>
+    <cfRule type="cellIs" dxfId="9" priority="28" operator="equal">
+      <formula>"Canceled"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
-      <formula>"high"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
-      <formula>"high"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
-      <formula>"highest"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
-      <formula>"low"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
-      <formula>"medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"high"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
-      <formula>"high"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
-      <formula>"highest"</formula>
+    <cfRule type="cellIs" dxfId="8" priority="29" operator="equal">
+      <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A2" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>